<commit_message>
Few changes in Wiley suite and driver module
</commit_message>
<xml_diff>
--- a/PPE_Prod_Smoke_Testing/Test Data/Automation_Datasheet.xlsx
+++ b/PPE_Prod_Smoke_Testing/Test Data/Automation_Datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\PPE_Prod_Smoke_Testing\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD084F4-6773-4D12-A141-7AD6077BAE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B394FA92-BB4C-4C96-A24F-144821ED2E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VET_Test_Data" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="302">
   <si>
     <t>Test_Case</t>
   </si>
@@ -725,9 +725,6 @@
     <t>NewLastName</t>
   </si>
   <si>
-    <t>autoags20230331051643@yopmail.com</t>
-  </si>
-  <si>
     <t>VET_Homepage_URL</t>
   </si>
   <si>
@@ -737,9 +734,6 @@
     <t>https://vetconsult.wiley.com/login/</t>
   </si>
   <si>
-    <t>autovet20230403113358@yopmail.com</t>
-  </si>
-  <si>
     <t>https://vetconsult.wiley.com/subscription</t>
   </si>
   <si>
@@ -813,6 +807,144 @@
   </si>
   <si>
     <t>Product_Search_Results_Page_Facet_Validation</t>
+  </si>
+  <si>
+    <t>Cart_Page_UI_Validation</t>
+  </si>
+  <si>
+    <t>Architecture%3A+Form%2C+Space%2C+and+Order%2C+5th+Edition-p-9781119853374</t>
+  </si>
+  <si>
+    <t>Login_Page_Validation</t>
+  </si>
+  <si>
+    <t>9781119820994</t>
+  </si>
+  <si>
+    <t>Add_Digital_Product_to_cart_for_New_User</t>
+  </si>
+  <si>
+    <t>California+Dreaming-p-9781119838371</t>
+  </si>
+  <si>
+    <t>testuser007788@yopmail.com</t>
+  </si>
+  <si>
+    <t>64108 Doral Dr</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Desert Hot Springs</t>
+  </si>
+  <si>
+    <t>92240</t>
+  </si>
+  <si>
+    <t>Add_Physical_Product_With_Guest_User</t>
+  </si>
+  <si>
+    <t>Model+Based+System+Architecture%2C+2nd+Edition-p-9781119746652</t>
+  </si>
+  <si>
+    <t>34 Edson St</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>Brockton</t>
+  </si>
+  <si>
+    <t>02302</t>
+  </si>
+  <si>
+    <t>Add_Physical_product_ForExistingUser</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Wiley_Cart_Page_URL</t>
+  </si>
+  <si>
+    <t>https://www.wiley.com/en-us/cart</t>
+  </si>
+  <si>
+    <t>Wiley</t>
+  </si>
+  <si>
+    <t>Shipping_Charge_For_Multiple_Products</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Brazil,American Samoa</t>
+  </si>
+  <si>
+    <t>Shipping_And_BillingAddresses_different</t>
+  </si>
+  <si>
+    <t>First+Farmers%3A+The+Origins+of+Agricultural+Societies%2C+2nd+Edition-p-9781119706342</t>
+  </si>
+  <si>
+    <t>TC23</t>
+  </si>
+  <si>
+    <t>Add_Coupon_To_Cart</t>
+  </si>
+  <si>
+    <t>4 Tideview Path</t>
+  </si>
+  <si>
+    <t>Plymouth</t>
+  </si>
+  <si>
+    <t>02360</t>
+  </si>
+  <si>
+    <t>TC24</t>
+  </si>
+  <si>
+    <t>VAT_Toltip_For_Asian_Countries</t>
+  </si>
+  <si>
+    <t>First+Farmers:+The+Origins+of+Agricultural+Societies,+2nd+Edition-p-9781119706342</t>
+  </si>
+  <si>
+    <t>cn,kr</t>
+  </si>
+  <si>
+    <t>VAT_Tooltip_Text</t>
+  </si>
+  <si>
+    <t>中国客户请向本地团队咨询中国销售价格</t>
+  </si>
+  <si>
+    <t>Expected_Result</t>
+  </si>
+  <si>
+    <t>Generic_info_hover_text_EBook_PDP</t>
+  </si>
+  <si>
+    <t>To download and read E-books offered from Wiley.com, you will access either Wiley Reader or the VitalSource Bookshelf Software.</t>
+  </si>
+  <si>
+    <t>us,gb</t>
+  </si>
+  <si>
+    <t>autovet20230404012133@yopmail.com</t>
+  </si>
+  <si>
+    <t>autoags20230404012438@yopmail.com</t>
+  </si>
+  <si>
+    <t>TC25</t>
+  </si>
+  <si>
+    <t>A+Companion+to+Ancient+Agriculture-p-9781118970942,A+Companion+to+American+Agricultural+History-p-9781119632245,Dr+Math+Presents+More+Geometry%3A+Learning+Geometry+is+Easy%21+Just+Ask+Dr+Math-p-9780471697107</t>
   </si>
 </sst>
 </file>
@@ -1015,7 +1147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1134,6 +1266,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1159,7 +1313,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="2" applyProtection="1"/>
@@ -1300,6 +1454,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Excel Built-in Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1733,7 +1902,7 @@
         <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>232</v>
+        <v>298</v>
       </c>
       <c r="G3"/>
       <c r="H3" s="39" t="s">
@@ -1757,7 +1926,7 @@
       <c r="D4"/>
       <c r="E4"/>
       <c r="F4" t="s">
-        <v>232</v>
+        <v>298</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>18</v>
@@ -1783,7 +1952,7 @@
       <c r="D5"/>
       <c r="E5"/>
       <c r="F5" t="s">
-        <v>232</v>
+        <v>298</v>
       </c>
       <c r="G5"/>
       <c r="H5" s="5" t="s">
@@ -1809,7 +1978,7 @@
         <v>227</v>
       </c>
       <c r="F6" t="s">
-        <v>232</v>
+        <v>298</v>
       </c>
       <c r="G6"/>
       <c r="H6" s="5" t="s">
@@ -2024,7 +2193,7 @@
   <dimension ref="A1:AMI24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2049,7 +2218,7 @@
         <v>87</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2057,7 +2226,7 @@
         <v>72</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2126,10 +2295,10 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>229</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2137,7 +2306,7 @@
         <v>44</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2145,11 +2314,24 @@
         <v>45</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>233</v>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
+      <c r="A16" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="17" spans="2:1023" x14ac:dyDescent="0.25">
       <c r="B17" s="11"/>
@@ -3199,6 +3381,7 @@
     <hyperlink ref="B12" r:id="rId9" xr:uid="{801B4DED-7801-4318-97CD-098CA8619835}"/>
     <hyperlink ref="B13" r:id="rId10" xr:uid="{9FFB8320-7069-40BE-95DA-DDF143F76429}"/>
     <hyperlink ref="B14" r:id="rId11" xr:uid="{BB714A28-7693-4CDF-8224-3523B40370C7}"/>
+    <hyperlink ref="B15" r:id="rId12" xr:uid="{B89C3401-5989-4C15-BB0E-1D0E766D458C}"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="1.1437000000000002" bottom="1.1437000000000002" header="0.75000000000000011" footer="0.75000000000000011"/>
   <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -4596,7 +4779,7 @@
         <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>228</v>
+        <v>299</v>
       </c>
       <c r="G3"/>
       <c r="H3" s="39" t="s">
@@ -4620,7 +4803,7 @@
       <c r="D4"/>
       <c r="E4"/>
       <c r="F4" t="s">
-        <v>228</v>
+        <v>299</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>18</v>
@@ -4646,7 +4829,7 @@
       <c r="D5"/>
       <c r="E5"/>
       <c r="F5" t="s">
-        <v>228</v>
+        <v>299</v>
       </c>
       <c r="G5"/>
       <c r="H5" s="5" t="s">
@@ -4672,7 +4855,7 @@
         <v>227</v>
       </c>
       <c r="F6" t="s">
-        <v>228</v>
+        <v>299</v>
       </c>
       <c r="G6"/>
       <c r="H6" s="5" t="s">
@@ -7887,49 +8070,46 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A971892C-2C4E-4A5C-8FEA-71D28CFA993F}">
-  <dimension ref="A1:AMP16"/>
+  <dimension ref="A1:AML26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="C26" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="42" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="40.5" style="34" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="9.75" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="9.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="4.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="26.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="45.75" style="34" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="7.625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="19.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="20.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="15.875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11.625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="17.125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="11.75" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="10" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="19" max="19" width="4.125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="20" max="20" width="15.375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="10.375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="11.75" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="8.25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="7.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="16.5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="24" max="24" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="25" max="25" width="16.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="7.75" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="10.125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="3.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="10.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="13.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="10.875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="11.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="13.25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="13.875" style="34" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1030" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1026" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -7951,7 +8131,7 @@
       <c r="G1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="83" t="s">
         <v>71</v>
       </c>
       <c r="I1" s="26" t="s">
@@ -8006,26 +8186,20 @@
         <v>57</v>
       </c>
       <c r="Z1" s="22" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="AA1" s="22" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="AB1" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="AC1" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD1" s="22" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE1" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="AF1" s="22" t="s">
         <v>93</v>
       </c>
+      <c r="AC1" s="86" t="s">
+        <v>294</v>
+      </c>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
       <c r="AG1" s="18"/>
       <c r="AH1" s="18"/>
       <c r="AI1" s="18"/>
@@ -9020,26 +9194,22 @@
       <c r="AMJ1" s="18"/>
       <c r="AMK1" s="18"/>
       <c r="AML1" s="18"/>
-      <c r="AMM1" s="18"/>
-      <c r="AMN1" s="18"/>
-      <c r="AMO1" s="18"/>
-      <c r="AMP1" s="18"/>
-    </row>
-    <row r="2" spans="1:1030" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:1026" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D2" s="19"/>
       <c r="E2" s="19"/>
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="H2" s="27"/>
       <c r="I2" s="19"/>
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
@@ -9060,27 +9230,23 @@
       <c r="Z2" s="19"/>
       <c r="AA2" s="19"/>
       <c r="AB2" s="19"/>
-      <c r="AC2" s="19"/>
-      <c r="AD2" s="19"/>
-      <c r="AE2" s="19"/>
-      <c r="AF2" s="19"/>
-      <c r="AG2" s="19"/>
-    </row>
-    <row r="3" spans="1:1030" ht="15" x14ac:dyDescent="0.25">
+      <c r="AC2" s="27"/>
+    </row>
+    <row r="3" spans="1:1026" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
+      <c r="H3" s="27"/>
       <c r="I3" s="19"/>
       <c r="J3" s="19"/>
       <c r="K3" s="19"/>
@@ -9101,25 +9267,21 @@
       <c r="Z3" s="19"/>
       <c r="AA3" s="19"/>
       <c r="AB3" s="19"/>
-      <c r="AC3" s="19"/>
-      <c r="AD3" s="19"/>
-      <c r="AE3" s="19"/>
-      <c r="AF3" s="19"/>
-      <c r="AG3" s="19"/>
-    </row>
-    <row r="4" spans="1:1030" ht="15" x14ac:dyDescent="0.25">
+      <c r="AC3" s="27"/>
+    </row>
+    <row r="4" spans="1:1026" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C4" s="32"/>
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="19"/>
       <c r="J4" s="19"/>
       <c r="K4" s="19"/>
@@ -9140,27 +9302,23 @@
       <c r="Z4" s="19"/>
       <c r="AA4" s="19"/>
       <c r="AB4" s="19"/>
-      <c r="AC4" s="19"/>
-      <c r="AD4" s="19"/>
-      <c r="AE4" s="19"/>
-      <c r="AF4" s="19"/>
-      <c r="AG4" s="19"/>
-    </row>
-    <row r="5" spans="1:1030" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC4" s="27"/>
+    </row>
+    <row r="5" spans="1:1026" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
+      <c r="H5" s="27"/>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
       <c r="K5" s="19"/>
@@ -9181,27 +9339,23 @@
       <c r="Z5" s="19"/>
       <c r="AA5" s="19"/>
       <c r="AB5" s="19"/>
-      <c r="AC5" s="19"/>
-      <c r="AD5" s="19"/>
-      <c r="AE5" s="19"/>
-      <c r="AF5" s="19"/>
-      <c r="AG5" s="19"/>
-    </row>
-    <row r="6" spans="1:1030" ht="15" x14ac:dyDescent="0.25">
+      <c r="AC5" s="27"/>
+    </row>
+    <row r="6" spans="1:1026" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
       <c r="F6" s="19"/>
       <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
+      <c r="H6" s="27"/>
       <c r="I6" s="19"/>
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
@@ -9222,27 +9376,23 @@
       <c r="Z6" s="19"/>
       <c r="AA6" s="19"/>
       <c r="AB6" s="19"/>
-      <c r="AC6" s="19"/>
-      <c r="AD6" s="19"/>
-      <c r="AE6" s="19"/>
-      <c r="AF6" s="19"/>
-      <c r="AG6" s="19"/>
-    </row>
-    <row r="7" spans="1:1030" ht="15" x14ac:dyDescent="0.25">
+      <c r="AC6" s="27"/>
+    </row>
+    <row r="7" spans="1:1026" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
       <c r="F7" s="19"/>
       <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
+      <c r="H7" s="27"/>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
@@ -9263,27 +9413,23 @@
       <c r="Z7" s="19"/>
       <c r="AA7" s="19"/>
       <c r="AB7" s="19"/>
-      <c r="AC7" s="19"/>
-      <c r="AD7" s="19"/>
-      <c r="AE7" s="19"/>
-      <c r="AF7" s="19"/>
-      <c r="AG7" s="19"/>
-    </row>
-    <row r="8" spans="1:1030" ht="15" x14ac:dyDescent="0.25">
+      <c r="AC7" s="27"/>
+    </row>
+    <row r="8" spans="1:1026" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
+      <c r="H8" s="27"/>
       <c r="I8" s="19"/>
       <c r="J8" s="19"/>
       <c r="K8" s="19"/>
@@ -9303,28 +9449,24 @@
       <c r="Y8" s="19"/>
       <c r="Z8" s="19"/>
       <c r="AA8" s="19"/>
-      <c r="AB8" s="19"/>
-      <c r="AC8" s="19"/>
-      <c r="AD8" s="19"/>
-      <c r="AE8" s="19"/>
-      <c r="AF8" s="19" t="s">
-        <v>246</v>
-      </c>
-      <c r="AG8" s="19"/>
-    </row>
-    <row r="9" spans="1:1030" ht="15" x14ac:dyDescent="0.25">
+      <c r="AB8" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="AC8" s="27"/>
+    </row>
+    <row r="9" spans="1:1026" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="19"/>
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
       <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
+      <c r="H9" s="27"/>
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
@@ -9345,25 +9487,21 @@
       <c r="Z9" s="19"/>
       <c r="AA9" s="19"/>
       <c r="AB9" s="19"/>
-      <c r="AC9" s="19"/>
-      <c r="AD9" s="19"/>
-      <c r="AE9" s="19"/>
-      <c r="AF9" s="19"/>
-      <c r="AG9" s="19"/>
-    </row>
-    <row r="10" spans="1:1030" ht="15" x14ac:dyDescent="0.25">
+      <c r="AC9" s="27"/>
+    </row>
+    <row r="10" spans="1:1026" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
+      <c r="H10" s="27"/>
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
@@ -9384,99 +9522,471 @@
       <c r="Z10" s="19"/>
       <c r="AA10" s="19"/>
       <c r="AB10" s="19"/>
-      <c r="AC10" s="19"/>
-      <c r="AD10" s="19"/>
-      <c r="AE10" s="19"/>
-      <c r="AF10" s="19"/>
-      <c r="AG10" s="19"/>
-    </row>
-    <row r="11" spans="1:1030" x14ac:dyDescent="0.2">
+      <c r="AC10" s="27"/>
+    </row>
+    <row r="11" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>32</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="C11" t="s">
-        <v>239</v>
-      </c>
-      <c r="H11" s="28"/>
+        <v>247</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="H11" s="84"/>
       <c r="I11" s="28"/>
       <c r="S11" s="28"/>
       <c r="T11" s="28"/>
-      <c r="AC11" s="28"/>
-      <c r="AD11" s="28"/>
-      <c r="AF11" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1030" x14ac:dyDescent="0.2">
+      <c r="Z11" s="28"/>
+      <c r="AB11" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>251</v>
-      </c>
-      <c r="C12" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1030" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>252</v>
-      </c>
-      <c r="C13" t="s">
-        <v>239</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1030" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>35</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>253</v>
-      </c>
-      <c r="C14" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1030" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="C15" t="s">
-        <v>239</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1030" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1026" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="81" t="s">
+        <v>255</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="C17" s="64" t="s">
         <v>257</v>
       </c>
-      <c r="C16" t="s">
-        <v>239</v>
-      </c>
-      <c r="AF16" t="s">
-        <v>246</v>
+    </row>
+    <row r="18" spans="1:29" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="82" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="80" t="s">
+        <v>258</v>
+      </c>
+      <c r="C18" s="64" t="s">
+        <v>257</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="H18" s="85" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A19" s="82" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="80" t="s">
+        <v>260</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>261</v>
+      </c>
+      <c r="D19" t="s">
+        <v>277</v>
+      </c>
+      <c r="E19" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="T19" t="s">
+        <v>263</v>
+      </c>
+      <c r="U19" t="s">
+        <v>75</v>
+      </c>
+      <c r="V19" t="s">
+        <v>264</v>
+      </c>
+      <c r="W19" t="s">
+        <v>265</v>
+      </c>
+      <c r="X19" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="Y19" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="82" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="80" t="s">
+        <v>267</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="D20" t="s">
+        <v>277</v>
+      </c>
+      <c r="E20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" t="s">
+        <v>269</v>
+      </c>
+      <c r="K20" t="s">
+        <v>75</v>
+      </c>
+      <c r="L20" t="s">
+        <v>270</v>
+      </c>
+      <c r="M20" t="s">
+        <v>271</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="P20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="R20" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="S20" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="82" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="80" t="s">
+        <v>273</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="D21" t="s">
+        <v>277</v>
+      </c>
+      <c r="E21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="J21" t="s">
+        <v>269</v>
+      </c>
+      <c r="K21" t="s">
+        <v>75</v>
+      </c>
+      <c r="L21" t="s">
+        <v>270</v>
+      </c>
+      <c r="M21" t="s">
+        <v>271</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="P21" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q21" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="R21" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="S21" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="82" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="80" t="s">
+        <v>278</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="D22" t="s">
+        <v>277</v>
+      </c>
+      <c r="E22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="K22" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="B23" s="80" t="s">
+        <v>281</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="D23" t="s">
+        <v>277</v>
+      </c>
+      <c r="E23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" t="s">
+        <v>269</v>
+      </c>
+      <c r="K23" t="s">
+        <v>75</v>
+      </c>
+      <c r="L23" t="s">
+        <v>270</v>
+      </c>
+      <c r="M23" t="s">
+        <v>271</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="P23" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q23" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="T23" t="s">
+        <v>263</v>
+      </c>
+      <c r="U23" t="s">
+        <v>75</v>
+      </c>
+      <c r="V23" t="s">
+        <v>264</v>
+      </c>
+      <c r="W23" t="s">
+        <v>265</v>
+      </c>
+      <c r="X23" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="Y23" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="82" t="s">
+        <v>283</v>
+      </c>
+      <c r="B24" s="80" t="s">
+        <v>284</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="D24" t="s">
+        <v>277</v>
+      </c>
+      <c r="E24" t="s">
+        <v>58</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" t="s">
+        <v>285</v>
+      </c>
+      <c r="K24" t="s">
+        <v>75</v>
+      </c>
+      <c r="L24" t="s">
+        <v>270</v>
+      </c>
+      <c r="M24" t="s">
+        <v>286</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="O24" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="P24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q24" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="R24" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="S24" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:29" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="82" t="s">
+        <v>288</v>
+      </c>
+      <c r="B25" s="80" t="s">
+        <v>289</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>291</v>
+      </c>
+      <c r="H25" s="34" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" ht="156.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="82" t="s">
+        <v>300</v>
+      </c>
+      <c r="B26" s="80" t="s">
+        <v>295</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>297</v>
+      </c>
+      <c r="H26" s="34" t="s">
+        <v>301</v>
+      </c>
+      <c r="AC26" s="34" t="s">
+        <v>296</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F18" r:id="rId1" xr:uid="{D027B8E7-40AC-49E0-8E74-B2AEBC8E87E7}"/>
+    <hyperlink ref="G18" r:id="rId2" xr:uid="{B9411EBE-CEDD-4625-8FC9-9E4794045FA4}"/>
+    <hyperlink ref="G19" r:id="rId3" xr:uid="{F4AABA22-0A1A-4D66-90C3-985611DF5848}"/>
+    <hyperlink ref="G20" r:id="rId4" xr:uid="{5AC18282-53C0-45EF-ADBB-4BEDDA5D06C8}"/>
+    <hyperlink ref="F21" r:id="rId5" xr:uid="{D1B7E816-5E8F-4086-8CEE-126B6F21E0BC}"/>
+    <hyperlink ref="G21" r:id="rId6" xr:uid="{65BD0EFF-BAD2-4613-B0C5-A4455613C13E}"/>
+    <hyperlink ref="G22" r:id="rId7" xr:uid="{341D9247-2D0B-4A64-87D9-235CAFCE42C8}"/>
+    <hyperlink ref="F22" r:id="rId8" xr:uid="{ED622E12-2F52-4698-9113-2ECDF2D7598D}"/>
+    <hyperlink ref="G23" r:id="rId9" xr:uid="{A6F7957B-788F-43E7-9455-67C33AC99EE5}"/>
+    <hyperlink ref="G24" r:id="rId10" xr:uid="{AD8E6186-29AA-40C5-966E-7ADC1D98BC00}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>